<commit_message>
0.1.21 New version with bipolar supply
 - poligons modified
 - top layer ia modified
 - GPIO is deleted
 - LED added
</commit_message>
<xml_diff>
--- a/Project Outputs for dv_cm/BOM/dv_cm.xlsx
+++ b/Project Outputs for dv_cm/BOM/dv_cm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\YandexDisk2\YandexDisk\OAI_NSU\Altium_projects\KVV\dv_cm\Project Outputs for dv_cm\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelemeshko-OAI\YandexDisk\OAI_NSU\Altium_projects\KVV\dv_cm\Project Outputs for dv_cm\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="16950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26115" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="dv_cm" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>Designator</t>
   </si>
@@ -197,30 +197,30 @@
     <t>2к</t>
   </si>
   <si>
-    <t>R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R60, R61, R62, R63</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>R15</t>
   </si>
   <si>
     <t>100к</t>
   </si>
   <si>
-    <t>R3, R5</t>
+    <t>R6, R7</t>
+  </si>
+  <si>
+    <t>2k4</t>
+  </si>
+  <si>
+    <t>R4, R8, R9, R10, R11, R12, R13, R14, R31, R32, R34, R36, R39</t>
+  </si>
+  <si>
+    <t>1к</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R5, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R60, R61, R62, R63</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>R1, R2, R7, R8, R9, R10, R11, R12, R13, R14, R31, R32, R34, R36, R39</t>
-  </si>
-  <si>
-    <t>1к</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -242,6 +242,18 @@
     <t>ОСМ ГК108-П-18ГС-3-10М</t>
   </si>
   <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Светодиод</t>
+  </si>
+  <si>
+    <t>SMD-LED</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
     <t>C14, C17, C21, C25, C33, C39, C41, C43, C45</t>
   </si>
   <si>
@@ -263,7 +275,7 @@
     <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C46, C47, C48, C49</t>
   </si>
   <si>
-    <t>1мкФ</t>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -323,16 +335,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -613,10 +619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -629,501 +632,517 @@
     <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>8</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1">
         <v>2</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1">
         <v>2</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1">
         <v>4</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1">
         <v>4</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1">
         <v>3</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="1">
         <v>4</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="4">
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="B22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1">
+        <v>13</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="1">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="1">
+        <v>24</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="1">
         <v>14</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="4">
-        <v>15</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="4">
-        <v>9</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="4">
-        <v>24</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="4">
-        <v>14</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>78</v>
+      <c r="E31" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>